<commit_message>
update linear fig based on Alex's suggestion
</commit_message>
<xml_diff>
--- a/stat/stats.xlsx
+++ b/stat/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au686295\Documents\GitHub\PhD\topography-control-of-ice-albedo\stat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88F533A6-1304-4344-99E5-9C1374790040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3D08FB-F11B-41F7-A7D6-700016615BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40575" yWindow="5415" windowWidth="22605" windowHeight="12360" xr2:uid="{ABE177B4-A381-4848-9D74-5AD89FAA9339}"/>
+    <workbookView xWindow="2076" yWindow="2268" windowWidth="17280" windowHeight="8976" xr2:uid="{ABE177B4-A381-4848-9D74-5AD89FAA9339}"/>
   </bookViews>
   <sheets>
     <sheet name="SW" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="11">
   <si>
     <t>slope</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>margin</t>
+  </si>
+  <si>
+    <t>inland</t>
   </si>
 </sst>
 </file>
@@ -103,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -119,6 +125,9 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,30 +443,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9078488-3FF1-45EB-8644-A617BC84D08D}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="6"/>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="6"/>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="6"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -471,8 +502,34 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -488,8 +545,38 @@
       <c r="E3" s="5">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.88</v>
+      </c>
+      <c r="K3" s="5">
+        <v>-0.77</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>-0.17</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -505,8 +592,38 @@
       <c r="E4" s="5">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0.86</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -522,8 +639,38 @@
       <c r="E5" s="5">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="4">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.53</v>
+      </c>
+      <c r="K5" s="5">
+        <v>-0.67</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="4">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -539,8 +686,38 @@
       <c r="E6" s="5">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>-0.63</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="K6" s="5">
+        <v>-0.56000000000000005</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -556,11 +733,45 @@
       <c r="E7" s="5">
         <v>0.53</v>
       </c>
+      <c r="H7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="K7" s="5">
+        <v>-0.49</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0.26</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="R7" s="5">
+        <v>0.96</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="Q1:R1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -573,20 +784,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -601,7 +812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -618,7 +829,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -635,7 +846,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -652,7 +863,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -669,7 +880,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>

</xml_diff>